<commit_message>
Most of CPU planned out
</commit_message>
<xml_diff>
--- a/Other/Digikey 3.3v parts.xlsx
+++ b/Other/Digikey 3.3v parts.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/John/Documents/MAX7000CPU-GEN3/Other/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Libraries\Documents\MAX7000CPU-GEN3\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB9A924-BD7E-9348-9371-7CD72B8461A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6937B77E-3ECF-42A6-849B-E1D61978325B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="1000" windowWidth="25040" windowHeight="13540" xr2:uid="{C9473B8E-9C9D-E34F-B67B-D30706104920}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{C9473B8E-9C9D-E34F-B67B-D30706104920}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -168,9 +168,6 @@
     <t>1.65 - 5.5 V</t>
   </si>
   <si>
-    <t>Xilinx CPLD 52 I/O</t>
-  </si>
-  <si>
     <t>https://www.digikey.com.au/en/products/detail/xilinx-inc/XC9572XL-10VQG64C/826991</t>
   </si>
   <si>
@@ -190,13 +187,22 @@
   </si>
   <si>
     <t>TQFP-100</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com.au/en/products/detail/ftdi-future-technology-devices-international-ltd/FT245RL-REEL/1836389</t>
+  </si>
+  <si>
+    <t>USB serial controller</t>
+  </si>
+  <si>
+    <t>Xilinx CPLD 72 I/O</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -211,12 +217,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF444444"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -247,12 +247,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -568,26 +567,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{431C1574-4FAC-CD4A-84A8-E26AB513194F}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.625" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="23.33203125" customWidth="1"/>
+    <col min="7" max="7" width="23.375" customWidth="1"/>
     <col min="8" max="8" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -619,19 +618,19 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0.53280000000000005</v>
+        <v>0.53200000000000003</v>
       </c>
       <c r="C3">
         <v>25</v>
       </c>
       <c r="D3">
         <f>B3*C3</f>
-        <v>13.320000000000002</v>
+        <v>13.3</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -653,10 +652,10 @@
       </c>
       <c r="L3">
         <f>SUM(D3:D24)</f>
-        <v>60.430000000000007</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+        <v>51.146000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -667,7 +666,7 @@
         <v>25</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D23" si="0">B4*C4</f>
+        <f t="shared" ref="D4:D5" si="0">B4*C4</f>
         <v>12.3</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -686,7 +685,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -694,11 +693,11 @@
         <v>0.66200000000000003</v>
       </c>
       <c r="C5">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>9.93</v>
+        <v>5.2960000000000003</v>
       </c>
       <c r="E5" t="s">
         <v>17</v>
@@ -719,7 +718,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -727,11 +726,11 @@
         <v>1.59</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <f>B6*C6</f>
-        <v>3.18</v>
+        <v>1.59</v>
       </c>
       <c r="E6" t="s">
         <v>26</v>
@@ -752,7 +751,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -773,7 +772,7 @@
         <v>34</v>
       </c>
       <c r="H7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I7">
         <v>0.5</v>
@@ -782,7 +781,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -790,11 +789,11 @@
         <v>1.52</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <f>B8*C8</f>
-        <v>4.5600000000000005</v>
+        <v>1.52</v>
       </c>
       <c r="E8" t="s">
         <v>42</v>
@@ -815,9 +814,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9">
         <v>6.73</v>
@@ -830,45 +829,53 @@
         <v>6.73</v>
       </c>
       <c r="E9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" t="s">
         <v>45</v>
       </c>
-      <c r="F9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" t="s">
-        <v>46</v>
-      </c>
       <c r="H9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H10" s="3"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" t="s">
         <v>51</v>
       </c>
-      <c r="I9" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="J9" t="s">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H10" s="4"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Circuit Board Drafted (it could probably be improved)
</commit_message>
<xml_diff>
--- a/Other/Digikey 3.3v parts.xlsx
+++ b/Other/Digikey 3.3v parts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Libraries\Documents\MAX7000CPU-GEN3\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C65B9F-CBB4-42F9-A03B-620A80561A2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAF1DED-363A-46BE-BCEB-C27D789717D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{C9473B8E-9C9D-E34F-B67B-D30706104920}"/>
   </bookViews>
@@ -579,7 +579,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -708,7 +708,7 @@
         <f t="shared" si="0"/>
         <v>5.2960000000000003</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F5" t="s">
@@ -907,6 +907,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E5" r:id="rId1" xr:uid="{7DADC605-86EF-4AB4-8F05-1FC1099FB55B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>